<commit_message>
chore: clean up unused files and dead code
Removed files:
- Root directory clutter: txt, xlsx, pdf, sql dump files
- Root markdown files: AGENTS.md, PERSONA_FIELDS_IMPLEMENTATION_STATE.md, etc.
- docs/ duplicates: PHASE2 planning documents, DATABASE_SCHEMA_DUMP_NEW.sql
- Unused components: performance-debug, coming-soon-page, gantt views
- Unused utilities: subscription-calculations.ts, excel-exporter.ts
- Debug scripts: inspect-data, test-aggregation, verify-dashboard-data, etc.
- Backup file: test-certificate-webhook.ts.bak

Total: 37 files removed (~56k lines of dead code/docs)

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/datamigration/05_Introducer_Commissions.xlsx
+++ b/datamigration/05_Introducer_Commissions.xlsx
@@ -523,7 +523,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Anand Sethia</t>
+          <t>Setcap</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -563,7 +563,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Anand Sethia</t>
+          <t>Setcap</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -11723,7 +11723,7 @@
       </c>
       <c r="B283" t="inlineStr">
         <is>
-          <t>Anand Sethia</t>
+          <t>Setcap</t>
         </is>
       </c>
       <c r="C283" t="inlineStr">
@@ -11763,7 +11763,7 @@
       </c>
       <c r="B284" t="inlineStr">
         <is>
-          <t>Anand Sethia</t>
+          <t>Setcap</t>
         </is>
       </c>
       <c r="C284" t="inlineStr">
@@ -13683,7 +13683,7 @@
       </c>
       <c r="B332" t="inlineStr">
         <is>
-          <t>Rick + Andrew</t>
+          <t>Altras Capital Financing Broker</t>
         </is>
       </c>
       <c r="C332" t="inlineStr">
@@ -13723,7 +13723,7 @@
       </c>
       <c r="B333" t="inlineStr">
         <is>
-          <t>Rick + Andrew</t>
+          <t>Altras Capital Financing Broker</t>
         </is>
       </c>
       <c r="C333" t="inlineStr">
@@ -15523,7 +15523,7 @@
       </c>
       <c r="B378" t="inlineStr">
         <is>
-          <t>Anand</t>
+          <t>Setcap</t>
         </is>
       </c>
       <c r="C378" t="inlineStr">
@@ -15563,7 +15563,7 @@
       </c>
       <c r="B379" t="inlineStr">
         <is>
-          <t>Anand</t>
+          <t>Setcap</t>
         </is>
       </c>
       <c r="C379" t="inlineStr">
@@ -15603,7 +15603,7 @@
       </c>
       <c r="B380" t="inlineStr">
         <is>
-          <t>Anand</t>
+          <t>Setcap</t>
         </is>
       </c>
       <c r="C380" t="inlineStr">
@@ -15643,7 +15643,7 @@
       </c>
       <c r="B381" t="inlineStr">
         <is>
-          <t>Anand</t>
+          <t>Setcap</t>
         </is>
       </c>
       <c r="C381" t="inlineStr">
@@ -15683,7 +15683,7 @@
       </c>
       <c r="B382" t="inlineStr">
         <is>
-          <t>Anand</t>
+          <t>Setcap</t>
         </is>
       </c>
       <c r="C382" t="inlineStr">
@@ -15723,7 +15723,7 @@
       </c>
       <c r="B383" t="inlineStr">
         <is>
-          <t>Anand</t>
+          <t>Setcap</t>
         </is>
       </c>
       <c r="C383" t="inlineStr">
@@ -15763,7 +15763,7 @@
       </c>
       <c r="B384" t="inlineStr">
         <is>
-          <t>Anand</t>
+          <t>Setcap</t>
         </is>
       </c>
       <c r="C384" t="inlineStr">
@@ -15803,7 +15803,7 @@
       </c>
       <c r="B385" t="inlineStr">
         <is>
-          <t>Anand</t>
+          <t>Setcap</t>
         </is>
       </c>
       <c r="C385" t="inlineStr">
@@ -15843,7 +15843,7 @@
       </c>
       <c r="B386" t="inlineStr">
         <is>
-          <t>Anand</t>
+          <t>Setcap</t>
         </is>
       </c>
       <c r="C386" t="inlineStr">
@@ -15883,7 +15883,7 @@
       </c>
       <c r="B387" t="inlineStr">
         <is>
-          <t>Anand</t>
+          <t>Setcap</t>
         </is>
       </c>
       <c r="C387" t="inlineStr">
@@ -15923,7 +15923,7 @@
       </c>
       <c r="B388" t="inlineStr">
         <is>
-          <t>Anand</t>
+          <t>Setcap</t>
         </is>
       </c>
       <c r="C388" t="inlineStr">
@@ -15963,7 +15963,7 @@
       </c>
       <c r="B389" t="inlineStr">
         <is>
-          <t>Anand</t>
+          <t>Setcap</t>
         </is>
       </c>
       <c r="C389" t="inlineStr">
@@ -16003,7 +16003,7 @@
       </c>
       <c r="B390" t="inlineStr">
         <is>
-          <t>Anand</t>
+          <t>Setcap</t>
         </is>
       </c>
       <c r="C390" t="inlineStr">
@@ -16043,7 +16043,7 @@
       </c>
       <c r="B391" t="inlineStr">
         <is>
-          <t>Anand</t>
+          <t>Setcap</t>
         </is>
       </c>
       <c r="C391" t="inlineStr">
@@ -16083,7 +16083,7 @@
       </c>
       <c r="B392" t="inlineStr">
         <is>
-          <t>Anand</t>
+          <t>Setcap</t>
         </is>
       </c>
       <c r="C392" t="inlineStr">
@@ -16123,7 +16123,7 @@
       </c>
       <c r="B393" t="inlineStr">
         <is>
-          <t>Dan</t>
+          <t>Daniel Baumslag</t>
         </is>
       </c>
       <c r="C393" t="inlineStr">
@@ -16163,7 +16163,7 @@
       </c>
       <c r="B394" t="inlineStr">
         <is>
-          <t>Dan</t>
+          <t>Daniel Baumslag</t>
         </is>
       </c>
       <c r="C394" t="inlineStr">
@@ -16203,7 +16203,7 @@
       </c>
       <c r="B395" t="inlineStr">
         <is>
-          <t>Dan</t>
+          <t>Daniel Baumslag</t>
         </is>
       </c>
       <c r="C395" t="inlineStr">
@@ -16243,7 +16243,7 @@
       </c>
       <c r="B396" t="inlineStr">
         <is>
-          <t>Dan</t>
+          <t>Daniel Baumslag</t>
         </is>
       </c>
       <c r="C396" t="inlineStr">
@@ -16283,7 +16283,7 @@
       </c>
       <c r="B397" t="inlineStr">
         <is>
-          <t>Dan</t>
+          <t>Daniel Baumslag</t>
         </is>
       </c>
       <c r="C397" t="inlineStr">
@@ -16323,7 +16323,7 @@
       </c>
       <c r="B398" t="inlineStr">
         <is>
-          <t>Dan</t>
+          <t>Daniel Baumslag</t>
         </is>
       </c>
       <c r="C398" t="inlineStr">
@@ -16363,7 +16363,7 @@
       </c>
       <c r="B399" t="inlineStr">
         <is>
-          <t>Dan</t>
+          <t>Daniel Baumslag</t>
         </is>
       </c>
       <c r="C399" t="inlineStr">
@@ -16403,7 +16403,7 @@
       </c>
       <c r="B400" t="inlineStr">
         <is>
-          <t>Dan</t>
+          <t>Daniel Baumslag</t>
         </is>
       </c>
       <c r="C400" t="inlineStr">
@@ -16443,7 +16443,7 @@
       </c>
       <c r="B401" t="inlineStr">
         <is>
-          <t>Dan</t>
+          <t>Daniel Baumslag</t>
         </is>
       </c>
       <c r="C401" t="inlineStr">
@@ -16483,7 +16483,7 @@
       </c>
       <c r="B402" t="inlineStr">
         <is>
-          <t>Dan</t>
+          <t>Daniel Baumslag</t>
         </is>
       </c>
       <c r="C402" t="inlineStr">
@@ -16523,7 +16523,7 @@
       </c>
       <c r="B403" t="inlineStr">
         <is>
-          <t>Dan</t>
+          <t>Daniel Baumslag</t>
         </is>
       </c>
       <c r="C403" t="inlineStr">
@@ -16563,7 +16563,7 @@
       </c>
       <c r="B404" t="inlineStr">
         <is>
-          <t>Dan</t>
+          <t>Daniel Baumslag</t>
         </is>
       </c>
       <c r="C404" t="inlineStr">
@@ -16603,7 +16603,7 @@
       </c>
       <c r="B405" t="inlineStr">
         <is>
-          <t>Dan</t>
+          <t>Daniel Baumslag</t>
         </is>
       </c>
       <c r="C405" t="inlineStr">
@@ -16643,7 +16643,7 @@
       </c>
       <c r="B406" t="inlineStr">
         <is>
-          <t>Dan</t>
+          <t>Daniel Baumslag</t>
         </is>
       </c>
       <c r="C406" t="inlineStr">
@@ -16683,7 +16683,7 @@
       </c>
       <c r="B407" t="inlineStr">
         <is>
-          <t>Dan</t>
+          <t>Daniel Baumslag</t>
         </is>
       </c>
       <c r="C407" t="inlineStr">
@@ -16723,7 +16723,7 @@
       </c>
       <c r="B408" t="inlineStr">
         <is>
-          <t>Dan</t>
+          <t>Daniel Baumslag</t>
         </is>
       </c>
       <c r="C408" t="inlineStr">
@@ -16763,7 +16763,7 @@
       </c>
       <c r="B409" t="inlineStr">
         <is>
-          <t>Dan</t>
+          <t>Daniel Baumslag</t>
         </is>
       </c>
       <c r="C409" t="inlineStr">
@@ -16803,7 +16803,7 @@
       </c>
       <c r="B410" t="inlineStr">
         <is>
-          <t>Dan</t>
+          <t>Daniel Baumslag</t>
         </is>
       </c>
       <c r="C410" t="inlineStr">
@@ -16843,7 +16843,7 @@
       </c>
       <c r="B411" t="inlineStr">
         <is>
-          <t>Dan</t>
+          <t>Daniel Baumslag</t>
         </is>
       </c>
       <c r="C411" t="inlineStr">
@@ -19083,7 +19083,7 @@
       </c>
       <c r="B467" t="inlineStr">
         <is>
-          <t>Dan</t>
+          <t>Daniel Baumslag</t>
         </is>
       </c>
       <c r="C467" t="inlineStr">
@@ -19123,7 +19123,7 @@
       </c>
       <c r="B468" t="inlineStr">
         <is>
-          <t>Dan</t>
+          <t>Daniel Baumslag</t>
         </is>
       </c>
       <c r="C468" t="inlineStr">
@@ -19163,7 +19163,7 @@
       </c>
       <c r="B469" t="inlineStr">
         <is>
-          <t>Dan</t>
+          <t>Daniel Baumslag</t>
         </is>
       </c>
       <c r="C469" t="inlineStr">
@@ -19203,7 +19203,7 @@
       </c>
       <c r="B470" t="inlineStr">
         <is>
-          <t>Dan</t>
+          <t>Daniel Baumslag</t>
         </is>
       </c>
       <c r="C470" t="inlineStr">
@@ -19243,7 +19243,7 @@
       </c>
       <c r="B471" t="inlineStr">
         <is>
-          <t>Dan</t>
+          <t>Daniel Baumslag</t>
         </is>
       </c>
       <c r="C471" t="inlineStr">
@@ -19283,7 +19283,7 @@
       </c>
       <c r="B472" t="inlineStr">
         <is>
-          <t>Dan</t>
+          <t>Daniel Baumslag</t>
         </is>
       </c>
       <c r="C472" t="inlineStr">
@@ -19323,7 +19323,7 @@
       </c>
       <c r="B473" t="inlineStr">
         <is>
-          <t>Dan</t>
+          <t>Daniel Baumslag</t>
         </is>
       </c>
       <c r="C473" t="inlineStr">
@@ -19363,7 +19363,7 @@
       </c>
       <c r="B474" t="inlineStr">
         <is>
-          <t>Dan</t>
+          <t>Daniel Baumslag</t>
         </is>
       </c>
       <c r="C474" t="inlineStr">
@@ -19403,7 +19403,7 @@
       </c>
       <c r="B475" t="inlineStr">
         <is>
-          <t>Dan</t>
+          <t>Daniel Baumslag</t>
         </is>
       </c>
       <c r="C475" t="inlineStr">
@@ -19443,7 +19443,7 @@
       </c>
       <c r="B476" t="inlineStr">
         <is>
-          <t>Dan</t>
+          <t>Daniel Baumslag</t>
         </is>
       </c>
       <c r="C476" t="inlineStr">
@@ -19483,7 +19483,7 @@
       </c>
       <c r="B477" t="inlineStr">
         <is>
-          <t>Dan</t>
+          <t>Daniel Baumslag</t>
         </is>
       </c>
       <c r="C477" t="inlineStr">
@@ -19523,7 +19523,7 @@
       </c>
       <c r="B478" t="inlineStr">
         <is>
-          <t>Dan</t>
+          <t>Daniel Baumslag</t>
         </is>
       </c>
       <c r="C478" t="inlineStr">
@@ -19883,7 +19883,7 @@
       </c>
       <c r="B487" t="inlineStr">
         <is>
-          <t>Dan</t>
+          <t>Daniel Baumslag</t>
         </is>
       </c>
       <c r="C487" t="inlineStr">
@@ -19923,7 +19923,7 @@
       </c>
       <c r="B488" t="inlineStr">
         <is>
-          <t>Dan</t>
+          <t>Daniel Baumslag</t>
         </is>
       </c>
       <c r="C488" t="inlineStr">
@@ -19963,7 +19963,7 @@
       </c>
       <c r="B489" t="inlineStr">
         <is>
-          <t>Dan</t>
+          <t>Daniel Baumslag</t>
         </is>
       </c>
       <c r="C489" t="inlineStr">
@@ -20003,7 +20003,7 @@
       </c>
       <c r="B490" t="inlineStr">
         <is>
-          <t>Dan</t>
+          <t>Daniel Baumslag</t>
         </is>
       </c>
       <c r="C490" t="inlineStr">
@@ -20043,7 +20043,7 @@
       </c>
       <c r="B491" t="inlineStr">
         <is>
-          <t>Dan</t>
+          <t>Daniel Baumslag</t>
         </is>
       </c>
       <c r="C491" t="inlineStr">
@@ -20083,7 +20083,7 @@
       </c>
       <c r="B492" t="inlineStr">
         <is>
-          <t>Dan</t>
+          <t>Daniel Baumslag</t>
         </is>
       </c>
       <c r="C492" t="inlineStr">
@@ -20123,7 +20123,7 @@
       </c>
       <c r="B493" t="inlineStr">
         <is>
-          <t>Dan</t>
+          <t>Daniel Baumslag</t>
         </is>
       </c>
       <c r="C493" t="inlineStr">
@@ -20603,7 +20603,7 @@
       </c>
       <c r="B505" t="inlineStr">
         <is>
-          <t>Anand</t>
+          <t>Setcap</t>
         </is>
       </c>
       <c r="C505" t="inlineStr">
@@ -20643,7 +20643,7 @@
       </c>
       <c r="B506" t="inlineStr">
         <is>
-          <t>Anand</t>
+          <t>Setcap</t>
         </is>
       </c>
       <c r="C506" t="inlineStr">
@@ -20683,7 +20683,7 @@
       </c>
       <c r="B507" t="inlineStr">
         <is>
-          <t>Anand</t>
+          <t>Setcap</t>
         </is>
       </c>
       <c r="C507" t="inlineStr">
@@ -20723,7 +20723,7 @@
       </c>
       <c r="B508" t="inlineStr">
         <is>
-          <t>Anand</t>
+          <t>Setcap</t>
         </is>
       </c>
       <c r="C508" t="inlineStr">
@@ -20763,7 +20763,7 @@
       </c>
       <c r="B509" t="inlineStr">
         <is>
-          <t>Anand</t>
+          <t>Setcap</t>
         </is>
       </c>
       <c r="C509" t="inlineStr">
@@ -20803,7 +20803,7 @@
       </c>
       <c r="B510" t="inlineStr">
         <is>
-          <t>Anand</t>
+          <t>Setcap</t>
         </is>
       </c>
       <c r="C510" t="inlineStr">
@@ -20843,7 +20843,7 @@
       </c>
       <c r="B511" t="inlineStr">
         <is>
-          <t>Anand</t>
+          <t>Setcap</t>
         </is>
       </c>
       <c r="C511" t="inlineStr">
@@ -20883,7 +20883,7 @@
       </c>
       <c r="B512" t="inlineStr">
         <is>
-          <t>Anand</t>
+          <t>Setcap</t>
         </is>
       </c>
       <c r="C512" t="inlineStr">
@@ -20923,7 +20923,7 @@
       </c>
       <c r="B513" t="inlineStr">
         <is>
-          <t>Anand</t>
+          <t>Setcap</t>
         </is>
       </c>
       <c r="C513" t="inlineStr">
@@ -20963,7 +20963,7 @@
       </c>
       <c r="B514" t="inlineStr">
         <is>
-          <t>Anand</t>
+          <t>Setcap</t>
         </is>
       </c>
       <c r="C514" t="inlineStr">
@@ -21003,7 +21003,7 @@
       </c>
       <c r="B515" t="inlineStr">
         <is>
-          <t>Anand</t>
+          <t>Setcap</t>
         </is>
       </c>
       <c r="C515" t="inlineStr">
@@ -21043,7 +21043,7 @@
       </c>
       <c r="B516" t="inlineStr">
         <is>
-          <t>Anand</t>
+          <t>Setcap</t>
         </is>
       </c>
       <c r="C516" t="inlineStr">
@@ -21083,7 +21083,7 @@
       </c>
       <c r="B517" t="inlineStr">
         <is>
-          <t>Anand</t>
+          <t>Setcap</t>
         </is>
       </c>
       <c r="C517" t="inlineStr">
@@ -21123,7 +21123,7 @@
       </c>
       <c r="B518" t="inlineStr">
         <is>
-          <t>Anand</t>
+          <t>Setcap</t>
         </is>
       </c>
       <c r="C518" t="inlineStr">
@@ -21163,7 +21163,7 @@
       </c>
       <c r="B519" t="inlineStr">
         <is>
-          <t>Anand</t>
+          <t>Setcap</t>
         </is>
       </c>
       <c r="C519" t="inlineStr">
@@ -21203,7 +21203,7 @@
       </c>
       <c r="B520" t="inlineStr">
         <is>
-          <t>Anand+Dan</t>
+          <t>Setcap+Daniel Baumslag</t>
         </is>
       </c>
       <c r="C520" t="inlineStr">
@@ -21243,7 +21243,7 @@
       </c>
       <c r="B521" t="inlineStr">
         <is>
-          <t>Anand+Dan</t>
+          <t>Setcap+Daniel Baumslag</t>
         </is>
       </c>
       <c r="C521" t="inlineStr">
@@ -22897,16 +22897,16 @@
         </is>
       </c>
       <c r="E562" t="n">
-        <v>25</v>
+        <v>500</v>
       </c>
       <c r="F562" t="inlineStr">
         <is>
-          <t>0.25</t>
+          <t>5.00</t>
         </is>
       </c>
       <c r="G562" t="inlineStr">
         <is>
-          <t>2500.00</t>
+          <t>50000.00</t>
         </is>
       </c>
       <c r="H562" t="inlineStr">

</xml_diff>